<commit_message>
QMM003 , QMM005 #3143
</commit_message>
<xml_diff>
--- a/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM003.xlsx
+++ b/nts.uk/uk.pr/pr.file/nts.uk.file.pr.infra/src/main/resources/report/QMM003.xlsx
@@ -229,7 +229,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="164" formatCode="0_);[Red]\(0\)"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -642,7 +642,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -44638,9 +44638,7 @@
   </sheetPr>
   <dimension ref="B2:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" zoomScalePageLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="12"/>
   <cols>
@@ -44721,7 +44719,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="9"/>
       <c r="J5" s="15"/>
-      <c r="K5" s="13"/>
+      <c r="K5" s="3"/>
       <c r="L5" s="18"/>
     </row>
     <row r="6" spans="2:12" ht="13.15" customHeight="1">
@@ -44734,7 +44732,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="11"/>
       <c r="J6" s="38"/>
-      <c r="K6" s="14"/>
+      <c r="K6" s="6"/>
       <c r="L6" s="20"/>
     </row>
     <row r="7" spans="2:12" ht="13.15" customHeight="1">
@@ -44747,7 +44745,7 @@
       <c r="H7" s="35"/>
       <c r="I7" s="8"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="13"/>
+      <c r="K7" s="3"/>
       <c r="L7" s="22"/>
     </row>
     <row r="8" spans="2:12" ht="13.15" customHeight="1">
@@ -44760,7 +44758,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="11"/>
       <c r="J8" s="38"/>
-      <c r="K8" s="14"/>
+      <c r="K8" s="6"/>
       <c r="L8" s="23"/>
     </row>
     <row r="9" spans="2:12" ht="13.15" customHeight="1">
@@ -44773,7 +44771,7 @@
       <c r="H9" s="35"/>
       <c r="I9" s="8"/>
       <c r="J9" s="4"/>
-      <c r="K9" s="13"/>
+      <c r="K9" s="3"/>
       <c r="L9" s="22"/>
     </row>
     <row r="10" spans="2:12" ht="13.15" customHeight="1">
@@ -44786,7 +44784,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="11"/>
       <c r="J10" s="5"/>
-      <c r="K10" s="14"/>
+      <c r="K10" s="6"/>
       <c r="L10" s="23"/>
     </row>
     <row r="11" spans="2:12" ht="13.15" customHeight="1">
@@ -44799,7 +44797,7 @@
       <c r="H11" s="35"/>
       <c r="I11" s="8"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="13"/>
+      <c r="K11" s="3"/>
       <c r="L11" s="22"/>
     </row>
     <row r="12" spans="2:12" ht="13.15" customHeight="1">
@@ -44812,7 +44810,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="11"/>
       <c r="J12" s="5"/>
-      <c r="K12" s="14"/>
+      <c r="K12" s="6"/>
       <c r="L12" s="23"/>
     </row>
     <row r="13" spans="2:12" ht="13.15" customHeight="1">
@@ -44825,7 +44823,7 @@
       <c r="H13" s="35"/>
       <c r="I13" s="8"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="13"/>
+      <c r="K13" s="3"/>
       <c r="L13" s="22"/>
     </row>
     <row r="14" spans="2:12" ht="13.15" customHeight="1">
@@ -44838,7 +44836,7 @@
       <c r="H14" s="5"/>
       <c r="I14" s="11"/>
       <c r="J14" s="5"/>
-      <c r="K14" s="14"/>
+      <c r="K14" s="6"/>
       <c r="L14" s="23"/>
     </row>
     <row r="15" spans="2:12" ht="13.15" customHeight="1">
@@ -44851,7 +44849,7 @@
       <c r="H15" s="35"/>
       <c r="I15" s="8"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="13"/>
+      <c r="K15" s="3"/>
       <c r="L15" s="22"/>
     </row>
     <row r="16" spans="2:12" ht="13.15" customHeight="1">
@@ -44864,7 +44862,7 @@
       <c r="H16" s="14"/>
       <c r="I16" s="11"/>
       <c r="J16" s="5"/>
-      <c r="K16" s="14"/>
+      <c r="K16" s="6"/>
       <c r="L16" s="23"/>
     </row>
     <row r="17" spans="2:12" ht="13.15" customHeight="1">
@@ -44877,7 +44875,7 @@
       <c r="H17" s="35"/>
       <c r="I17" s="8"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="13"/>
+      <c r="K17" s="3"/>
       <c r="L17" s="22"/>
     </row>
     <row r="18" spans="2:12" ht="13.15" customHeight="1">
@@ -44890,7 +44888,7 @@
       <c r="H18" s="7"/>
       <c r="I18" s="11"/>
       <c r="J18" s="5"/>
-      <c r="K18" s="14"/>
+      <c r="K18" s="6"/>
       <c r="L18" s="23"/>
     </row>
     <row r="19" spans="2:12" ht="13.15" customHeight="1">
@@ -44903,7 +44901,7 @@
       <c r="H19" s="13"/>
       <c r="I19" s="8"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="36"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="28"/>
     </row>
     <row r="20" spans="2:12" ht="13.15" customHeight="1">
@@ -44916,7 +44914,7 @@
       <c r="H20" s="14"/>
       <c r="I20" s="11"/>
       <c r="J20" s="5"/>
-      <c r="K20" s="14"/>
+      <c r="K20" s="6"/>
       <c r="L20" s="23"/>
     </row>
     <row r="21" spans="2:12" ht="13.15" customHeight="1">
@@ -44929,7 +44927,7 @@
       <c r="H21" s="13"/>
       <c r="I21" s="9"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="13"/>
+      <c r="K21" s="3"/>
       <c r="L21" s="22"/>
     </row>
     <row r="22" spans="2:12" ht="13.15" customHeight="1">
@@ -44942,7 +44940,7 @@
       <c r="H22" s="14"/>
       <c r="I22" s="11"/>
       <c r="J22" s="5"/>
-      <c r="K22" s="14"/>
+      <c r="K22" s="6"/>
       <c r="L22" s="23"/>
     </row>
     <row r="23" spans="2:12" ht="13.15" customHeight="1">
@@ -44955,7 +44953,7 @@
       <c r="H23" s="13"/>
       <c r="I23" s="9"/>
       <c r="J23" s="2"/>
-      <c r="K23" s="13"/>
+      <c r="K23" s="3"/>
       <c r="L23" s="22"/>
     </row>
     <row r="24" spans="2:12" ht="13.15" customHeight="1">
@@ -44968,7 +44966,7 @@
       <c r="H24" s="14"/>
       <c r="I24" s="11"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="14"/>
+      <c r="K24" s="6"/>
       <c r="L24" s="23"/>
     </row>
     <row r="25" spans="2:12" ht="13.15" customHeight="1">
@@ -44981,7 +44979,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="9"/>
       <c r="J25" s="2"/>
-      <c r="K25" s="13"/>
+      <c r="K25" s="3"/>
       <c r="L25" s="22"/>
     </row>
     <row r="26" spans="2:12" ht="13.15" customHeight="1">
@@ -44994,7 +44992,7 @@
       <c r="H26" s="14"/>
       <c r="I26" s="11"/>
       <c r="J26" s="5"/>
-      <c r="K26" s="14"/>
+      <c r="K26" s="6"/>
       <c r="L26" s="23"/>
     </row>
     <row r="27" spans="2:12" ht="13.15" customHeight="1">
@@ -45007,7 +45005,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="9"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="13"/>
+      <c r="K27" s="3"/>
       <c r="L27" s="22"/>
     </row>
     <row r="28" spans="2:12" ht="13.15" customHeight="1">
@@ -45020,7 +45018,7 @@
       <c r="H28" s="14"/>
       <c r="I28" s="11"/>
       <c r="J28" s="5"/>
-      <c r="K28" s="14"/>
+      <c r="K28" s="6"/>
       <c r="L28" s="23"/>
     </row>
     <row r="29" spans="2:12" ht="13.15" customHeight="1">
@@ -45033,7 +45031,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="9"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="13"/>
+      <c r="K29" s="3"/>
       <c r="L29" s="22"/>
     </row>
     <row r="30" spans="2:12" ht="13.15" customHeight="1">
@@ -45046,7 +45044,7 @@
       <c r="H30" s="14"/>
       <c r="I30" s="11"/>
       <c r="J30" s="5"/>
-      <c r="K30" s="14"/>
+      <c r="K30" s="6"/>
       <c r="L30" s="23"/>
     </row>
     <row r="31" spans="2:12" ht="13.15" customHeight="1">
@@ -45059,7 +45057,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="9"/>
       <c r="J31" s="2"/>
-      <c r="K31" s="13"/>
+      <c r="K31" s="3"/>
       <c r="L31" s="22"/>
     </row>
     <row r="32" spans="2:12" ht="13.15" customHeight="1">
@@ -45072,7 +45070,7 @@
       <c r="H32" s="14"/>
       <c r="I32" s="11"/>
       <c r="J32" s="5"/>
-      <c r="K32" s="14"/>
+      <c r="K32" s="6"/>
       <c r="L32" s="23"/>
     </row>
     <row r="33" spans="2:12" ht="13.15" customHeight="1">
@@ -45085,7 +45083,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="9"/>
       <c r="J33" s="2"/>
-      <c r="K33" s="13"/>
+      <c r="K33" s="3"/>
       <c r="L33" s="22"/>
     </row>
     <row r="34" spans="2:12" ht="13.15" customHeight="1">
@@ -45098,7 +45096,7 @@
       <c r="H34" s="14"/>
       <c r="I34" s="11"/>
       <c r="J34" s="5"/>
-      <c r="K34" s="14"/>
+      <c r="K34" s="6"/>
       <c r="L34" s="23"/>
     </row>
     <row r="35" spans="2:12" ht="13.15" customHeight="1">
@@ -45111,7 +45109,7 @@
       <c r="H35" s="13"/>
       <c r="I35" s="9"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="13"/>
+      <c r="K35" s="3"/>
       <c r="L35" s="22"/>
     </row>
     <row r="36" spans="2:12" ht="13.15" customHeight="1">
@@ -45124,7 +45122,7 @@
       <c r="H36" s="14"/>
       <c r="I36" s="11"/>
       <c r="J36" s="5"/>
-      <c r="K36" s="14"/>
+      <c r="K36" s="6"/>
       <c r="L36" s="23"/>
     </row>
     <row r="37" spans="2:12" ht="13.15" customHeight="1">
@@ -45137,7 +45135,7 @@
       <c r="H37" s="13"/>
       <c r="I37" s="9"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="13"/>
+      <c r="K37" s="3"/>
       <c r="L37" s="22"/>
     </row>
     <row r="38" spans="2:12" ht="13.15" customHeight="1">
@@ -45150,7 +45148,7 @@
       <c r="H38" s="14"/>
       <c r="I38" s="11"/>
       <c r="J38" s="5"/>
-      <c r="K38" s="14"/>
+      <c r="K38" s="6"/>
       <c r="L38" s="23"/>
     </row>
     <row r="39" spans="2:12" ht="13.15" customHeight="1">
@@ -45163,7 +45161,7 @@
       <c r="H39" s="13"/>
       <c r="I39" s="9"/>
       <c r="J39" s="2"/>
-      <c r="K39" s="13"/>
+      <c r="K39" s="3"/>
       <c r="L39" s="22"/>
     </row>
     <row r="40" spans="2:12" ht="13.15" customHeight="1">
@@ -45176,7 +45174,7 @@
       <c r="H40" s="14"/>
       <c r="I40" s="11"/>
       <c r="J40" s="5"/>
-      <c r="K40" s="14"/>
+      <c r="K40" s="6"/>
       <c r="L40" s="23"/>
     </row>
     <row r="41" spans="2:12" ht="13.15" customHeight="1">
@@ -45189,7 +45187,7 @@
       <c r="H41" s="13"/>
       <c r="I41" s="9"/>
       <c r="J41" s="2"/>
-      <c r="K41" s="13"/>
+      <c r="K41" s="3"/>
       <c r="L41" s="22"/>
     </row>
     <row r="42" spans="2:12" ht="13.15" customHeight="1">
@@ -45202,7 +45200,7 @@
       <c r="H42" s="14"/>
       <c r="I42" s="11"/>
       <c r="J42" s="5"/>
-      <c r="K42" s="14"/>
+      <c r="K42" s="6"/>
       <c r="L42" s="23"/>
     </row>
     <row r="43" spans="2:12" ht="13.15" customHeight="1">
@@ -45215,7 +45213,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="9"/>
       <c r="J43" s="2"/>
-      <c r="K43" s="13"/>
+      <c r="K43" s="3"/>
       <c r="L43" s="22"/>
     </row>
     <row r="44" spans="2:12" ht="13.15" customHeight="1">
@@ -45228,7 +45226,7 @@
       <c r="H44" s="14"/>
       <c r="I44" s="11"/>
       <c r="J44" s="5"/>
-      <c r="K44" s="14"/>
+      <c r="K44" s="6"/>
       <c r="L44" s="23"/>
     </row>
     <row r="45" spans="2:12" ht="13.15" customHeight="1">
@@ -45241,7 +45239,7 @@
       <c r="H45" s="13"/>
       <c r="I45" s="9"/>
       <c r="J45" s="2"/>
-      <c r="K45" s="13"/>
+      <c r="K45" s="3"/>
       <c r="L45" s="22"/>
     </row>
     <row r="46" spans="2:12" ht="13.15" customHeight="1">
@@ -45254,7 +45252,7 @@
       <c r="H46" s="14"/>
       <c r="I46" s="11"/>
       <c r="J46" s="5"/>
-      <c r="K46" s="14"/>
+      <c r="K46" s="6"/>
       <c r="L46" s="23"/>
     </row>
     <row r="47" spans="2:12" ht="13.15" customHeight="1">
@@ -45267,7 +45265,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="9"/>
       <c r="J47" s="2"/>
-      <c r="K47" s="13"/>
+      <c r="K47" s="3"/>
       <c r="L47" s="22"/>
     </row>
     <row r="48" spans="2:12" ht="13.15" customHeight="1">
@@ -45280,7 +45278,7 @@
       <c r="H48" s="14"/>
       <c r="I48" s="11"/>
       <c r="J48" s="5"/>
-      <c r="K48" s="14"/>
+      <c r="K48" s="6"/>
       <c r="L48" s="23"/>
     </row>
     <row r="49" spans="2:12" ht="13.15" customHeight="1">
@@ -45293,7 +45291,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="9"/>
       <c r="J49" s="2"/>
-      <c r="K49" s="13"/>
+      <c r="K49" s="3"/>
       <c r="L49" s="22"/>
     </row>
     <row r="50" spans="2:12" ht="13.15" customHeight="1">
@@ -45306,7 +45304,7 @@
       <c r="H50" s="14"/>
       <c r="I50" s="11"/>
       <c r="J50" s="5"/>
-      <c r="K50" s="14"/>
+      <c r="K50" s="6"/>
       <c r="L50" s="23"/>
     </row>
     <row r="51" spans="2:12" ht="13.15" customHeight="1">
@@ -45319,7 +45317,7 @@
       <c r="H51" s="36"/>
       <c r="I51" s="27"/>
       <c r="J51" s="39"/>
-      <c r="K51" s="36"/>
+      <c r="K51" s="26"/>
       <c r="L51" s="28"/>
     </row>
     <row r="52" spans="2:12" ht="13.15" customHeight="1">
@@ -45332,7 +45330,7 @@
       <c r="H52" s="14"/>
       <c r="I52" s="11"/>
       <c r="J52" s="5"/>
-      <c r="K52" s="14"/>
+      <c r="K52" s="6"/>
       <c r="L52" s="23"/>
     </row>
     <row r="53" spans="2:12" ht="13.15" customHeight="1" thickBot="1">
@@ -45345,7 +45343,7 @@
       <c r="H53" s="37"/>
       <c r="I53" s="32"/>
       <c r="J53" s="40"/>
-      <c r="K53" s="37"/>
+      <c r="K53" s="31"/>
       <c r="L53" s="33"/>
     </row>
   </sheetData>
@@ -45363,7 +45361,7 @@
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.2" right="0.2" top="0.75" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="70" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"ＭＳ ゴシック,Regular"&amp;10日通システム株式会社  &amp;C&amp;"ＭＳ ゴシック,Regular"&amp;16住民税納付先の登録 &amp;R&amp;"ＭＳ ゴシック,Regular"&amp;10&amp;KFF0000 &amp;K01+000     &amp;D　&amp;T　
 &amp;KFF0000 &amp;K01+000          page&amp;P</oddHeader>

</xml_diff>